<commit_message>
sắp hoàn thiện giao diện admin và user
</commit_message>
<xml_diff>
--- a/dataset/data_doanhthubapnuoc.xlsx
+++ b/dataset/data_doanhthubapnuoc.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\DoAnCuoiKy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7DEFD30-3D78-4810-8DA3-3AC2D388C953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -37,50 +31,50 @@
     <t>Doanh thu</t>
   </si>
   <si>
+    <t>Tháng 12/2024</t>
+  </si>
+  <si>
+    <t>Tháng 1/2025</t>
+  </si>
+  <si>
     <t>Tháng 2/2025</t>
   </si>
   <si>
-    <t>Tháng 12/2024</t>
-  </si>
-  <si>
-    <t>Tháng 1/2025</t>
-  </si>
-  <si>
     <t>Tháng 3/2025</t>
   </si>
   <si>
+    <t>Poca Wavy 54gr</t>
+  </si>
+  <si>
+    <t>Khoai Tây Lay's Stax</t>
+  </si>
+  <si>
+    <t>Snack Thái</t>
+  </si>
+  <si>
+    <t>Coke Zero 32oz</t>
+  </si>
+  <si>
+    <t>Coke 32oz</t>
+  </si>
+  <si>
+    <t>2 Coke + 1 Bắp (Phô Mai, Caramel)</t>
+  </si>
+  <si>
+    <t>1 Coke + 1 Bắp (Phô Mai, Caramel)</t>
+  </si>
+  <si>
     <t>1 Bắp Phô Mai</t>
   </si>
   <si>
-    <t>1 Coke + 1 Bắp (Phô Mai, Caramel)</t>
-  </si>
-  <si>
-    <t>2 Coke + 1 Bắp (Phô Mai, Caramel)</t>
-  </si>
-  <si>
-    <t>Coke 32oz</t>
-  </si>
-  <si>
-    <t>Coke Zero 32oz</t>
-  </si>
-  <si>
-    <t>Snack Thái</t>
-  </si>
-  <si>
-    <t>Khoai Tây Lay's Stax</t>
-  </si>
-  <si>
     <t>Poca Khoai Tây</t>
-  </si>
-  <si>
-    <t>Poca Wavy 54gr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,21 +137,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,7 +181,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -229,7 +215,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -264,10 +249,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -440,21 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="14.53125" customWidth="1"/>
-    <col min="2" max="2" width="29.46484375" customWidth="1"/>
-    <col min="3" max="3" width="12.53125" customWidth="1"/>
-    <col min="4" max="4" width="16.9296875" customWidth="1"/>
-    <col min="5" max="5" width="11.265625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -479,16 +456,16 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>75000</v>
+        <v>28000</v>
       </c>
       <c r="D2">
-        <v>332</v>
+        <v>266</v>
       </c>
       <c r="E2">
-        <v>24900000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>7448000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -496,16 +473,16 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>119000</v>
+        <v>59000</v>
       </c>
       <c r="D3">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="E3">
-        <v>20349000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>11800000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -513,16 +490,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>179000</v>
+        <v>35000</v>
       </c>
       <c r="D4">
-        <v>313</v>
+        <v>410</v>
       </c>
       <c r="E4">
-        <v>56027000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>14350000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -533,13 +510,13 @@
         <v>39000</v>
       </c>
       <c r="D5">
-        <v>308</v>
+        <v>418</v>
       </c>
       <c r="E5">
-        <v>12012000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>16302000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -550,13 +527,13 @@
         <v>39000</v>
       </c>
       <c r="D6">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="E6">
-        <v>7917000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>18408000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -564,16 +541,16 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>35000</v>
+        <v>179000</v>
       </c>
       <c r="D7">
-        <v>245</v>
+        <v>369</v>
       </c>
       <c r="E7">
-        <v>8575000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>66051000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -581,16 +558,16 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>59000</v>
+        <v>119000</v>
       </c>
       <c r="D8">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="E8">
-        <v>12685000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>20944000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -598,16 +575,16 @@
         <v>16</v>
       </c>
       <c r="C9">
-        <v>28000</v>
+        <v>75000</v>
       </c>
       <c r="D9">
-        <v>465</v>
+        <v>499</v>
       </c>
       <c r="E9">
-        <v>13020000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>37425000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -618,217 +595,217 @@
         <v>28000</v>
       </c>
       <c r="D10">
-        <v>387</v>
+        <v>186</v>
       </c>
       <c r="E10">
-        <v>10836000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>5208000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>75000</v>
+        <v>119000</v>
       </c>
       <c r="D11">
-        <v>499</v>
+        <v>163</v>
       </c>
       <c r="E11">
-        <v>37425000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>19397000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>119000</v>
+        <v>28000</v>
       </c>
       <c r="D12">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E12">
-        <v>20944000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>5208000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>179000</v>
+        <v>28000</v>
       </c>
       <c r="D13">
-        <v>369</v>
+        <v>298</v>
       </c>
       <c r="E13">
-        <v>66051000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <v>8344000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>39000</v>
+        <v>59000</v>
       </c>
       <c r="D14">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E14">
-        <v>18408000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>27612000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>39000</v>
+        <v>75000</v>
       </c>
       <c r="D15">
-        <v>418</v>
+        <v>497</v>
       </c>
       <c r="E15">
-        <v>16302000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <v>37275000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>35000</v>
+        <v>39000</v>
       </c>
       <c r="D16">
-        <v>410</v>
+        <v>264</v>
       </c>
       <c r="E16">
-        <v>14350000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>10296000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>59000</v>
+        <v>39000</v>
       </c>
       <c r="D17">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="E17">
-        <v>11800000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>6474000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>28000</v>
+        <v>179000</v>
       </c>
       <c r="D18">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="E18">
-        <v>5208000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>41170000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>28000</v>
+        <v>35000</v>
       </c>
       <c r="D19">
-        <v>266</v>
+        <v>341</v>
       </c>
       <c r="E19">
-        <v>7448000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>11935000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>75000</v>
+        <v>119000</v>
       </c>
       <c r="D20">
-        <v>497</v>
+        <v>171</v>
       </c>
       <c r="E20">
-        <v>37275000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>20349000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>119000</v>
+        <v>179000</v>
       </c>
       <c r="D21">
-        <v>163</v>
+        <v>313</v>
       </c>
       <c r="E21">
-        <v>19397000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>56027000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>179000</v>
+        <v>39000</v>
       </c>
       <c r="D22">
-        <v>230</v>
+        <v>308</v>
       </c>
       <c r="E22">
-        <v>41170000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>12012000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -839,64 +816,64 @@
         <v>39000</v>
       </c>
       <c r="D23">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="E23">
-        <v>6474000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+        <v>7917000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>39000</v>
+        <v>35000</v>
       </c>
       <c r="D24">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="E24">
-        <v>10296000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>8575000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C25">
-        <v>35000</v>
+        <v>28000</v>
       </c>
       <c r="D25">
-        <v>341</v>
+        <v>465</v>
       </c>
       <c r="E25">
-        <v>11935000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>13020000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>59000</v>
+        <v>28000</v>
       </c>
       <c r="D26">
-        <v>468</v>
+        <v>387</v>
       </c>
       <c r="E26">
-        <v>27612000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>10836000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -904,50 +881,50 @@
         <v>16</v>
       </c>
       <c r="C27">
-        <v>28000</v>
+        <v>75000</v>
       </c>
       <c r="D27">
-        <v>298</v>
+        <v>332</v>
       </c>
       <c r="E27">
-        <v>8344000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+        <v>24900000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>28000</v>
+        <v>59000</v>
       </c>
       <c r="D28">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="E28">
-        <v>5208000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+        <v>12685000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>75000</v>
+        <v>39000</v>
       </c>
       <c r="D29">
-        <v>187</v>
+        <v>495</v>
       </c>
       <c r="E29">
-        <v>14025000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+        <v>19305000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -955,16 +932,16 @@
         <v>10</v>
       </c>
       <c r="C30">
-        <v>119000</v>
+        <v>59000</v>
       </c>
       <c r="D30">
-        <v>167</v>
+        <v>417</v>
       </c>
       <c r="E30">
-        <v>19873000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+        <v>24603000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -972,16 +949,16 @@
         <v>11</v>
       </c>
       <c r="C31">
-        <v>179000</v>
+        <v>35000</v>
       </c>
       <c r="D31">
-        <v>395</v>
+        <v>294</v>
       </c>
       <c r="E31">
-        <v>70705000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+        <v>10290000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -992,30 +969,30 @@
         <v>39000</v>
       </c>
       <c r="D32">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="E32">
-        <v>19305000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+        <v>18447000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>39000</v>
+        <v>75000</v>
       </c>
       <c r="D33">
-        <v>473</v>
+        <v>187</v>
       </c>
       <c r="E33">
-        <v>18447000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+        <v>14025000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1023,16 +1000,16 @@
         <v>14</v>
       </c>
       <c r="C34">
-        <v>35000</v>
+        <v>179000</v>
       </c>
       <c r="D34">
-        <v>294</v>
+        <v>395</v>
       </c>
       <c r="E34">
-        <v>10290000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+        <v>70705000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1040,21 +1017,21 @@
         <v>15</v>
       </c>
       <c r="C35">
-        <v>59000</v>
+        <v>119000</v>
       </c>
       <c r="D35">
-        <v>417</v>
+        <v>167</v>
       </c>
       <c r="E35">
-        <v>24603000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+        <v>19873000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C36">
         <v>28000</v>
@@ -1066,12 +1043,12 @@
         <v>9436000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <v>28000</v>

</xml_diff>